<commit_message>
Updated Team Records.xlsx after Week 13
</commit_message>
<xml_diff>
--- a/Base/Excel Files/Team Records.xlsx
+++ b/Base/Excel Files/Team Records.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136736bc97bfa800/Robbie/Football/Simulation app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136736bc97bfa800/Robbie/Football/nfl-simulation-app/Base/Excel Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="783" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37CC3235-626A-4759-90FA-56F4EFE83DA3}"/>
+  <xr:revisionPtr revIDLastSave="848" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76D3F61D-3A36-4812-B04C-2AC22DCD021F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="81">
   <si>
     <t>Bills</t>
   </si>
@@ -135,9 +135,6 @@
     <t>1-0-0</t>
   </si>
   <si>
-    <t>1-1-0</t>
-  </si>
-  <si>
     <t>0-2-0</t>
   </si>
   <si>
@@ -156,15 +153,6 @@
     <t>2-2-0</t>
   </si>
   <si>
-    <t>3-0-0</t>
-  </si>
-  <si>
-    <t>2-4-0</t>
-  </si>
-  <si>
-    <t>5-1-0</t>
-  </si>
-  <si>
     <t>4-3-0</t>
   </si>
   <si>
@@ -195,48 +183,21 @@
     <t>2-5-0</t>
   </si>
   <si>
-    <t>7-4-0</t>
-  </si>
-  <si>
-    <t>4-7-0</t>
-  </si>
-  <si>
     <t>0-4-0</t>
   </si>
   <si>
     <t>2-6-0</t>
   </si>
   <si>
-    <t>6-5-0</t>
-  </si>
-  <si>
-    <t>8-3-0</t>
-  </si>
-  <si>
     <t>3-1-0</t>
   </si>
   <si>
-    <t>5-6-0</t>
-  </si>
-  <si>
-    <t>9-2-0</t>
-  </si>
-  <si>
     <t>4-0-0</t>
   </si>
   <si>
-    <t>0-10-1</t>
-  </si>
-  <si>
-    <t>0-7-0</t>
-  </si>
-  <si>
     <t>5-7-0</t>
   </si>
   <si>
-    <t>3-8-0</t>
-  </si>
-  <si>
     <t>3-6-0</t>
   </si>
   <si>
@@ -249,19 +210,64 @@
     <t>6-6-0</t>
   </si>
   <si>
-    <t>5-5-1</t>
-  </si>
-  <si>
-    <t>2-9-0</t>
-  </si>
-  <si>
     <t>9-3-0</t>
   </si>
   <si>
     <t>7-2-0</t>
   </si>
   <si>
-    <t>1-6-0</t>
+    <t>7-5-0</t>
+  </si>
+  <si>
+    <t>5-5-0</t>
+  </si>
+  <si>
+    <t>6-7-0</t>
+  </si>
+  <si>
+    <t>3-9-0</t>
+  </si>
+  <si>
+    <t>9-4-0</t>
+  </si>
+  <si>
+    <t>7-1-0</t>
+  </si>
+  <si>
+    <t>6-5-1</t>
+  </si>
+  <si>
+    <t>7-6-0</t>
+  </si>
+  <si>
+    <t>3-2-0</t>
+  </si>
+  <si>
+    <t>6-3-0</t>
+  </si>
+  <si>
+    <t>2-10-0</t>
+  </si>
+  <si>
+    <t>2-7-0</t>
+  </si>
+  <si>
+    <t>4-8-0</t>
+  </si>
+  <si>
+    <t>1-10-1</t>
+  </si>
+  <si>
+    <t>1-4-0</t>
+  </si>
+  <si>
+    <t>1-7-0</t>
+  </si>
+  <si>
+    <t>10-2-0</t>
+  </si>
+  <si>
+    <t>6-2-0</t>
   </si>
 </sst>
 </file>
@@ -590,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,6 +608,7 @@
     <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -709,201 +716,201 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>60</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W2" t="s">
-        <v>66</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>61</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>43</v>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="L3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="T3" t="s">
         <v>35</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" t="s">
-        <v>58</v>
+        <v>38</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="AB3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AC3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="AD3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG3" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -911,100 +918,100 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="K4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="O4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="W4" t="s">
-        <v>67</v>
+      <c r="W4" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="Y4" s="3" t="s">
         <v>46</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AD4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG4" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logged Week 15 and simulated Week 16
</commit_message>
<xml_diff>
--- a/Base/Excel Files/Team Records.xlsx
+++ b/Base/Excel Files/Team Records.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136736bc97bfa800/Robbie/Football/nfl-simulation-app/Base/Excel Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="848" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76D3F61D-3A36-4812-B04C-2AC22DCD021F}"/>
+  <xr:revisionPtr revIDLastSave="977" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D3B449-14C0-4310-9C47-A5CDCA60122F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>Bills</t>
   </si>
@@ -132,142 +132,118 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>1-0-0</t>
-  </si>
-  <si>
-    <t>0-2-0</t>
-  </si>
-  <si>
-    <t>2-0-0</t>
-  </si>
-  <si>
     <t>2-1-0</t>
   </si>
   <si>
-    <t>0-3-0</t>
-  </si>
-  <si>
     <t>1-3-0</t>
   </si>
   <si>
     <t>2-2-0</t>
   </si>
   <si>
-    <t>4-3-0</t>
-  </si>
-  <si>
-    <t>3-4-0</t>
-  </si>
-  <si>
-    <t>5-2-0</t>
-  </si>
-  <si>
     <t>1-2-0</t>
   </si>
   <si>
-    <t>4-4-0</t>
-  </si>
-  <si>
-    <t>5-3-0</t>
-  </si>
-  <si>
-    <t>3-5-0</t>
-  </si>
-  <si>
     <t>5-4-0</t>
   </si>
   <si>
-    <t>4-5-0</t>
-  </si>
-  <si>
-    <t>2-5-0</t>
-  </si>
-  <si>
-    <t>0-4-0</t>
-  </si>
-  <si>
-    <t>2-6-0</t>
-  </si>
-  <si>
     <t>3-1-0</t>
   </si>
   <si>
     <t>4-0-0</t>
   </si>
   <si>
-    <t>5-7-0</t>
-  </si>
-  <si>
     <t>3-6-0</t>
   </si>
   <si>
-    <t>8-4-0</t>
-  </si>
-  <si>
-    <t>6-1-0</t>
-  </si>
-  <si>
-    <t>6-6-0</t>
-  </si>
-  <si>
-    <t>9-3-0</t>
-  </si>
-  <si>
     <t>7-2-0</t>
   </si>
   <si>
-    <t>7-5-0</t>
-  </si>
-  <si>
     <t>5-5-0</t>
   </si>
   <si>
     <t>6-7-0</t>
   </si>
   <si>
-    <t>3-9-0</t>
-  </si>
-  <si>
-    <t>9-4-0</t>
-  </si>
-  <si>
-    <t>7-1-0</t>
-  </si>
-  <si>
-    <t>6-5-1</t>
-  </si>
-  <si>
-    <t>7-6-0</t>
-  </si>
-  <si>
     <t>3-2-0</t>
   </si>
   <si>
     <t>6-3-0</t>
   </si>
   <si>
-    <t>2-10-0</t>
-  </si>
-  <si>
     <t>2-7-0</t>
   </si>
   <si>
-    <t>4-8-0</t>
-  </si>
-  <si>
-    <t>1-10-1</t>
-  </si>
-  <si>
     <t>1-4-0</t>
   </si>
   <si>
-    <t>1-7-0</t>
-  </si>
-  <si>
-    <t>10-2-0</t>
-  </si>
-  <si>
-    <t>6-2-0</t>
+    <t>10-3-0</t>
+  </si>
+  <si>
+    <t>4-1-0</t>
+  </si>
+  <si>
+    <t>2-3-0</t>
+  </si>
+  <si>
+    <t>8-2-0</t>
+  </si>
+  <si>
+    <t>8-6-0</t>
+  </si>
+  <si>
+    <t>7-7-0</t>
+  </si>
+  <si>
+    <t>3-11-0</t>
+  </si>
+  <si>
+    <t>0-5-0</t>
+  </si>
+  <si>
+    <t>3-7-0</t>
+  </si>
+  <si>
+    <t>9-5-0</t>
+  </si>
+  <si>
+    <t>7-6-1</t>
+  </si>
+  <si>
+    <t>7-3-0</t>
+  </si>
+  <si>
+    <t>2-12-0</t>
+  </si>
+  <si>
+    <t>6-4-0</t>
+  </si>
+  <si>
+    <t>10-4-0</t>
+  </si>
+  <si>
+    <t>8-1-0</t>
+  </si>
+  <si>
+    <t>4-10-0</t>
+  </si>
+  <si>
+    <t>2-11-1</t>
+  </si>
+  <si>
+    <t>11-3-0</t>
+  </si>
+  <si>
+    <t>6-8-0</t>
+  </si>
+  <si>
+    <t>5-9-0</t>
+  </si>
+  <si>
+    <t>6-5-0</t>
+  </si>
+  <si>
+    <t>4-6-0</t>
   </si>
 </sst>
 </file>
@@ -596,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AG5" sqref="AG5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,100 +692,100 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="V2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="X2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="AC2" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -817,100 +793,100 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="S3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="W3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AA3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>37</v>
+        <v>52</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -918,100 +894,100 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="L4" s="3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG4" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logged Week 16 and performed season sim from Week 17
</commit_message>
<xml_diff>
--- a/Base/Excel Files/Team Records.xlsx
+++ b/Base/Excel Files/Team Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136736bc97bfa800/Robbie/Football/nfl-simulation-app/Base/Excel Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="977" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D3B449-14C0-4310-9C47-A5CDCA60122F}"/>
+  <xr:revisionPtr revIDLastSave="1051" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759357E7-3936-452A-8188-E486259899B1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
   <si>
     <t>Bills</t>
   </si>
@@ -132,54 +132,24 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>2-1-0</t>
-  </si>
-  <si>
     <t>1-3-0</t>
   </si>
   <si>
     <t>2-2-0</t>
   </si>
   <si>
-    <t>1-2-0</t>
-  </si>
-  <si>
-    <t>5-4-0</t>
-  </si>
-  <si>
     <t>3-1-0</t>
   </si>
   <si>
-    <t>4-0-0</t>
-  </si>
-  <si>
-    <t>3-6-0</t>
-  </si>
-  <si>
-    <t>7-2-0</t>
-  </si>
-  <si>
     <t>5-5-0</t>
   </si>
   <si>
-    <t>6-7-0</t>
-  </si>
-  <si>
     <t>3-2-0</t>
   </si>
   <si>
-    <t>6-3-0</t>
-  </si>
-  <si>
-    <t>2-7-0</t>
-  </si>
-  <si>
     <t>1-4-0</t>
   </si>
   <si>
-    <t>10-3-0</t>
-  </si>
-  <si>
     <t>4-1-0</t>
   </si>
   <si>
@@ -189,61 +159,79 @@
     <t>8-2-0</t>
   </si>
   <si>
-    <t>8-6-0</t>
-  </si>
-  <si>
-    <t>7-7-0</t>
-  </si>
-  <si>
-    <t>3-11-0</t>
-  </si>
-  <si>
     <t>0-5-0</t>
   </si>
   <si>
     <t>3-7-0</t>
   </si>
   <si>
-    <t>9-5-0</t>
-  </si>
-  <si>
-    <t>7-6-1</t>
-  </si>
-  <si>
     <t>7-3-0</t>
   </si>
   <si>
-    <t>2-12-0</t>
-  </si>
-  <si>
     <t>6-4-0</t>
   </si>
   <si>
-    <t>10-4-0</t>
-  </si>
-  <si>
-    <t>8-1-0</t>
-  </si>
-  <si>
-    <t>4-10-0</t>
-  </si>
-  <si>
-    <t>2-11-1</t>
-  </si>
-  <si>
-    <t>11-3-0</t>
-  </si>
-  <si>
-    <t>6-8-0</t>
-  </si>
-  <si>
-    <t>5-9-0</t>
-  </si>
-  <si>
     <t>6-5-0</t>
   </si>
   <si>
     <t>4-6-0</t>
+  </si>
+  <si>
+    <t>9-6-0</t>
+  </si>
+  <si>
+    <t>8-7-0</t>
+  </si>
+  <si>
+    <t>4-11-0</t>
+  </si>
+  <si>
+    <t>4-7-0</t>
+  </si>
+  <si>
+    <t>7-8-0</t>
+  </si>
+  <si>
+    <t>5-6-0</t>
+  </si>
+  <si>
+    <t>7-7-1</t>
+  </si>
+  <si>
+    <t>2-13-0</t>
+  </si>
+  <si>
+    <t>2-8-0</t>
+  </si>
+  <si>
+    <t>10-5-0</t>
+  </si>
+  <si>
+    <t>11-4-0</t>
+  </si>
+  <si>
+    <t>5-0-0</t>
+  </si>
+  <si>
+    <t>9-1-0</t>
+  </si>
+  <si>
+    <t>6-9-0</t>
+  </si>
+  <si>
+    <t>5-10-0</t>
+  </si>
+  <si>
+    <t>2-12-1</t>
+  </si>
+  <si>
+    <t>12-3-0</t>
+  </si>
+  <si>
+    <t>7-4-0</t>
+  </si>
+  <si>
+    <t>8-3-0</t>
   </si>
 </sst>
 </file>
@@ -573,7 +561,7 @@
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,100 +680,100 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>59</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -793,100 +781,100 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="V3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="AF3" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -894,100 +882,100 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="L4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="Y4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG4" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-simulated Week 17, factoring in more player injuries
</commit_message>
<xml_diff>
--- a/Base/Excel Files/Team Records.xlsx
+++ b/Base/Excel Files/Team Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136736bc97bfa800/Robbie/Football/nfl-simulation-app/Base/Excel Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1051" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759357E7-3936-452A-8188-E486259899B1}"/>
+  <xr:revisionPtr revIDLastSave="1117" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C677C64-50A0-430E-83E6-A1F329F64D27}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="62">
   <si>
     <t>Bills</t>
   </si>
@@ -132,18 +132,6 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>1-3-0</t>
-  </si>
-  <si>
-    <t>2-2-0</t>
-  </si>
-  <si>
-    <t>3-1-0</t>
-  </si>
-  <si>
-    <t>5-5-0</t>
-  </si>
-  <si>
     <t>3-2-0</t>
   </si>
   <si>
@@ -156,82 +144,73 @@
     <t>2-3-0</t>
   </si>
   <si>
-    <t>8-2-0</t>
-  </si>
-  <si>
     <t>0-5-0</t>
   </si>
   <si>
-    <t>3-7-0</t>
-  </si>
-  <si>
-    <t>7-3-0</t>
-  </si>
-  <si>
-    <t>6-4-0</t>
-  </si>
-  <si>
     <t>6-5-0</t>
   </si>
   <si>
-    <t>4-6-0</t>
-  </si>
-  <si>
-    <t>9-6-0</t>
-  </si>
-  <si>
-    <t>8-7-0</t>
-  </si>
-  <si>
-    <t>4-11-0</t>
-  </si>
-  <si>
     <t>4-7-0</t>
   </si>
   <si>
-    <t>7-8-0</t>
-  </si>
-  <si>
     <t>5-6-0</t>
   </si>
   <si>
-    <t>7-7-1</t>
-  </si>
-  <si>
-    <t>2-13-0</t>
-  </si>
-  <si>
-    <t>2-8-0</t>
-  </si>
-  <si>
-    <t>10-5-0</t>
-  </si>
-  <si>
-    <t>11-4-0</t>
-  </si>
-  <si>
     <t>5-0-0</t>
   </si>
   <si>
-    <t>9-1-0</t>
-  </si>
-  <si>
-    <t>6-9-0</t>
-  </si>
-  <si>
-    <t>5-10-0</t>
-  </si>
-  <si>
-    <t>2-12-1</t>
-  </si>
-  <si>
-    <t>12-3-0</t>
-  </si>
-  <si>
     <t>7-4-0</t>
   </si>
   <si>
     <t>8-3-0</t>
+  </si>
+  <si>
+    <t>10-6-0</t>
+  </si>
+  <si>
+    <t>8-8-0</t>
+  </si>
+  <si>
+    <t>4-12-0</t>
+  </si>
+  <si>
+    <t>7-9-0</t>
+  </si>
+  <si>
+    <t>8-7-1</t>
+  </si>
+  <si>
+    <t>9-7-0</t>
+  </si>
+  <si>
+    <t>2-14-0</t>
+  </si>
+  <si>
+    <t>2-9-0</t>
+  </si>
+  <si>
+    <t>11-5-0</t>
+  </si>
+  <si>
+    <t>3-8-0</t>
+  </si>
+  <si>
+    <t>9-2-0</t>
+  </si>
+  <si>
+    <t>6-10-0</t>
+  </si>
+  <si>
+    <t>2-13-1</t>
+  </si>
+  <si>
+    <t>13-3-0</t>
+  </si>
+  <si>
+    <t>12-4-0</t>
+  </si>
+  <si>
+    <t>5-11-0</t>
   </si>
 </sst>
 </file>
@@ -560,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
@@ -680,100 +659,100 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="L2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -781,100 +760,100 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="V3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>37</v>
       </c>
       <c r="Y3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="AF3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -882,100 +861,100 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="L4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="AG4" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simulated Wild Card round and logged it
</commit_message>
<xml_diff>
--- a/Base/Excel Files/Team Records.xlsx
+++ b/Base/Excel Files/Team Records.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136736bc97bfa800/Robbie/Football/nfl-simulation-app/Base/Excel Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1117" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C677C64-50A0-430E-83E6-A1F329F64D27}"/>
+  <xr:revisionPtr revIDLastSave="1219" documentId="11_F25DC773A252ABDACC1048E3A1D945EA5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43EA6AAC-5310-463C-BBD4-DB31AD940433}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>Bills</t>
   </si>
@@ -132,85 +132,88 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>3-2-0</t>
-  </si>
-  <si>
-    <t>1-4-0</t>
-  </si>
-  <si>
-    <t>4-1-0</t>
-  </si>
-  <si>
-    <t>2-3-0</t>
-  </si>
-  <si>
-    <t>0-5-0</t>
-  </si>
-  <si>
-    <t>6-5-0</t>
-  </si>
-  <si>
-    <t>4-7-0</t>
-  </si>
-  <si>
-    <t>5-6-0</t>
-  </si>
-  <si>
-    <t>5-0-0</t>
-  </si>
-  <si>
-    <t>7-4-0</t>
-  </si>
-  <si>
-    <t>8-3-0</t>
-  </si>
-  <si>
-    <t>10-6-0</t>
-  </si>
-  <si>
-    <t>8-8-0</t>
-  </si>
-  <si>
-    <t>4-12-0</t>
-  </si>
-  <si>
-    <t>7-9-0</t>
-  </si>
-  <si>
-    <t>8-7-1</t>
-  </si>
-  <si>
-    <t>9-7-0</t>
-  </si>
-  <si>
-    <t>2-14-0</t>
-  </si>
-  <si>
-    <t>2-9-0</t>
-  </si>
-  <si>
-    <t>11-5-0</t>
-  </si>
-  <si>
-    <t>3-8-0</t>
-  </si>
-  <si>
-    <t>9-2-0</t>
-  </si>
-  <si>
-    <t>6-10-0</t>
-  </si>
-  <si>
-    <t>2-13-1</t>
-  </si>
-  <si>
-    <t>13-3-0</t>
-  </si>
-  <si>
-    <t>12-4-0</t>
-  </si>
-  <si>
-    <t>5-11-0</t>
+    <t>11-6-0</t>
+  </si>
+  <si>
+    <t>5-1-0</t>
+  </si>
+  <si>
+    <t>7-5-0</t>
+  </si>
+  <si>
+    <t>9-8-0</t>
+  </si>
+  <si>
+    <t>4-2-0</t>
+  </si>
+  <si>
+    <t>6-6-0</t>
+  </si>
+  <si>
+    <t>4-13-0</t>
+  </si>
+  <si>
+    <t>0-6-0</t>
+  </si>
+  <si>
+    <t>4-8-0</t>
+  </si>
+  <si>
+    <t>10-7-0</t>
+  </si>
+  <si>
+    <t>3-3-0</t>
+  </si>
+  <si>
+    <t>8-4-0</t>
+  </si>
+  <si>
+    <t>8-9-0</t>
+  </si>
+  <si>
+    <t>5-7-0</t>
+  </si>
+  <si>
+    <t>1-5-0</t>
+  </si>
+  <si>
+    <t>9-7-1</t>
+  </si>
+  <si>
+    <t>3-14-0</t>
+  </si>
+  <si>
+    <t>3-9-0</t>
+  </si>
+  <si>
+    <t>12-5-0</t>
+  </si>
+  <si>
+    <t>7-10-0</t>
+  </si>
+  <si>
+    <t>6-0-0</t>
+  </si>
+  <si>
+    <t>10-2-0</t>
+  </si>
+  <si>
+    <t>2-4-0</t>
+  </si>
+  <si>
+    <t>6-11-0</t>
+  </si>
+  <si>
+    <t>3-13-1</t>
+  </si>
+  <si>
+    <t>13-4-0</t>
+  </si>
+  <si>
+    <t>9-3-0</t>
+  </si>
+  <si>
+    <t>5-12-0</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
@@ -548,7 +551,7 @@
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -659,22 +662,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>47</v>
@@ -683,76 +686,76 @@
         <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="U2" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="AE2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -760,100 +763,100 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="N3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="Y3" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -861,100 +864,100 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>56</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>